<commit_message>
new updates for split drive
</commit_message>
<xml_diff>
--- a/drive2_fsRIDL.xlsx
+++ b/drive2_fsRIDL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/078bf24b81d0bbc9/Dropbox_new/fsRIDL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/078bf24b81d0bbc9/Dropbox_new/suzukii_pop_supp_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{0EB1F4E7-C64C-4780-9AC9-BB6BA9933D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4143580A-2EE4-4E47-8B3A-ECDEAE179C66}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{0EB1F4E7-C64C-4780-9AC9-BB6BA9933D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{785C447E-EFFB-4B2C-A84F-CB34FE211614}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1950" windowWidth="15300" windowHeight="7965" xr2:uid="{42F50F30-6F04-40BD-A5D9-284346A8740A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{42F50F30-6F04-40BD-A5D9-284346A8740A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>AA</t>
   </si>
@@ -424,7 +424,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,11 +475,11 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>

</xml_diff>